<commit_message>
added code snippet styling and introduced padding into the blog
</commit_message>
<xml_diff>
--- a/content/sheets/alumni.xlsx
+++ b/content/sheets/alumni.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t xml:space="preserve">Anubhav Jain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jaya Sagar</t>
   </si>
 </sst>
 </file>
@@ -193,11 +196,11 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.48046875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.7"/>
@@ -310,7 +313,7 @@
     </row>
     <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>2016</v>

</xml_diff>

<commit_message>
Updated member page and .xlsx sheet
</commit_message>
<xml_diff>
--- a/content/sheets/alumni.xlsx
+++ b/content/sheets/alumni.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="30">
   <si>
     <t xml:space="preserve">name</t>
   </si>
@@ -65,6 +65,51 @@
   </si>
   <si>
     <t xml:space="preserve">Jaya Sagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vivek Gusain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marmik Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mayank Singh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mukul C. Mahadik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sumit Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Abhiraj Singh Rathore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Amol Bobade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Divyanshu Bhaik</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kunal Kishore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sahaj Kulshrestha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parthivi Jain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Varan Singh Rohila</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Achyut Sharma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Priyanka Kumar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rishi Kumar</t>
   </si>
 </sst>
 </file>
@@ -160,7 +205,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -175,6 +220,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -194,13 +243,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H9"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I22" activeCellId="0" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.5" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="22.7"/>
@@ -415,7 +464,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -438,6 +487,396 @@
         <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>2017</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>2021</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -467,6 +906,18 @@
     <hyperlink ref="E9" r:id="rId22" display="https://istenith.com/prody/"/>
     <hyperlink ref="F9" r:id="rId23" display="https://istenith.com/prody/"/>
     <hyperlink ref="G9" r:id="rId24" display="https://istenith.com/prody/"/>
+    <hyperlink ref="E10" r:id="rId25" display="https://istenith.com/prody/"/>
+    <hyperlink ref="F10" r:id="rId26" display="https://istenith.com/prody/"/>
+    <hyperlink ref="G10" r:id="rId27" display="https://istenith.com/prody/"/>
+    <hyperlink ref="E11" r:id="rId28" display="https://istenith.com/prody/"/>
+    <hyperlink ref="F11" r:id="rId29" display="https://istenith.com/prody/"/>
+    <hyperlink ref="G11" r:id="rId30" display="https://istenith.com/prody/"/>
+    <hyperlink ref="E12" r:id="rId31" display="https://istenith.com/prody/"/>
+    <hyperlink ref="F12" r:id="rId32" display="https://istenith.com/prody/"/>
+    <hyperlink ref="G12" r:id="rId33" display="https://istenith.com/prody/"/>
+    <hyperlink ref="E13" r:id="rId34" display="https://istenith.com/prody/"/>
+    <hyperlink ref="F13" r:id="rId35" display="https://istenith.com/prody/"/>
+    <hyperlink ref="G13" r:id="rId36" display="https://istenith.com/prody/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>